<commit_message>
Update 2p4. Added Simscape Multibody Magic Formula Tire for MATLAB R21b and higher.
</commit_message>
<xml_diff>
--- a/Libraries/Vehicle/Tire/Delft/sm_car_data_Tire_Delft.xlsx
+++ b/Libraries/Vehicle/Tire/Delft/sm_car_data_Tire_Delft.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\Others\smiller\ssvt\Libraries\Vehicle\Tire\Delft\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\smiller\simscape\demo\allsimscape\cars\vehicle-templates\Libraries\Vehicle\Tire\Delft\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E66743A-AFD8-478E-8504-DA04C8FD9C6A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A71B7BC-99CB-41F5-B517-C83D384AA440}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1812" yWindow="1836" windowWidth="20424" windowHeight="10212" activeTab="4" xr2:uid="{038AE485-2DF6-4480-A05B-AFF15F06FE64}"/>
+    <workbookView xWindow="5775" yWindow="2265" windowWidth="21600" windowHeight="12675" xr2:uid="{038AE485-2DF6-4480-A05B-AFF15F06FE64}"/>
   </bookViews>
   <sheets>
     <sheet name="Tir_235_50R24" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="34">
   <si>
     <t>Units</t>
   </si>
@@ -70,9 +70,6 @@
     <t>which('235-50R24_8jR24_280_kPa.tir')</t>
   </si>
   <si>
-    <t>Inertia</t>
-  </si>
-  <si>
     <t>roadFile</t>
   </si>
   <si>
@@ -131,6 +128,15 @@
   </si>
   <si>
     <t>which('Truck_430_50R38.tir')</t>
+  </si>
+  <si>
+    <t>mjRim</t>
+  </si>
+  <si>
+    <t>kg, kg*m^2</t>
+  </si>
+  <si>
+    <t>Rim [Mass, Ixx, Iyy]</t>
   </si>
 </sst>
 </file>
@@ -223,8 +229,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -240,11 +244,48 @@
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="15">
+  <dxfs count="20">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -665,22 +706,22 @@
   </sheetPr>
   <dimension ref="A1:AA26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" style="19" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" style="17" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
     <col min="6" max="8" width="10" customWidth="1"/>
-    <col min="9" max="15" width="6.6640625" customWidth="1"/>
+    <col min="9" max="15" width="6.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
@@ -700,7 +741,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -709,8 +750,8 @@
       <c r="E2" s="7"/>
       <c r="F2" s="7"/>
       <c r="G2" s="7"/>
-      <c r="H2" s="21" t="s">
-        <v>28</v>
+      <c r="H2" s="19" t="s">
+        <v>27</v>
       </c>
       <c r="I2"/>
       <c r="J2"/>
@@ -731,7 +772,7 @@
       <c r="Z2"/>
       <c r="AA2"/>
     </row>
-    <row r="3" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
@@ -740,7 +781,7 @@
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
       <c r="H3" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I3"/>
       <c r="J3"/>
@@ -761,7 +802,7 @@
       <c r="Z3"/>
       <c r="AA3"/>
     </row>
-    <row r="4" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>7</v>
       </c>
@@ -792,20 +833,20 @@
       <c r="Z4"/>
       <c r="AA4"/>
     </row>
-    <row r="5" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
       <c r="G5" s="13"/>
-      <c r="H5" s="20" t="s">
-        <v>29</v>
+      <c r="H5" s="18" t="s">
+        <v>28</v>
       </c>
       <c r="J5"/>
       <c r="K5"/>
       <c r="M5"/>
-      <c r="N5" s="20" t="s">
+      <c r="N5" s="18" t="s">
         <v>10</v>
       </c>
       <c r="O5"/>
@@ -822,49 +863,37 @@
       <c r="Z5"/>
       <c r="AA5"/>
     </row>
-    <row r="6" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
-      <c r="F6" s="15">
-        <v>10</v>
-      </c>
-      <c r="G6" s="16">
-        <v>1</v>
-      </c>
-      <c r="H6" s="16">
-        <v>2</v>
-      </c>
-      <c r="J6"/>
-      <c r="K6"/>
-      <c r="L6"/>
-      <c r="M6"/>
-      <c r="N6"/>
-      <c r="O6"/>
-      <c r="P6"/>
-      <c r="Q6"/>
-      <c r="R6"/>
-      <c r="S6"/>
-      <c r="T6"/>
-      <c r="U6"/>
-      <c r="V6"/>
-      <c r="W6"/>
-      <c r="X6"/>
-      <c r="Y6"/>
-      <c r="Z6"/>
-      <c r="AA6"/>
-    </row>
-    <row r="7" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" s="20">
+        <v>0</v>
+      </c>
+      <c r="G6" s="21">
+        <v>0</v>
+      </c>
+      <c r="H6" s="21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
       <c r="G7" s="13"/>
-      <c r="H7" s="20" t="s">
-        <v>13</v>
+      <c r="H7" s="18" t="s">
+        <v>12</v>
       </c>
       <c r="J7"/>
       <c r="K7"/>
@@ -885,15 +914,15 @@
       <c r="Z7"/>
       <c r="AA7"/>
     </row>
-    <row r="8" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
       <c r="G8" s="13"/>
-      <c r="H8" s="20" t="s">
-        <v>15</v>
+      <c r="H8" s="18" t="s">
+        <v>14</v>
       </c>
       <c r="J8"/>
       <c r="K8"/>
@@ -914,27 +943,27 @@
       <c r="Z8"/>
       <c r="AA8"/>
     </row>
-    <row r="9" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
       <c r="F9" s="13"/>
       <c r="G9" s="13"/>
       <c r="H9" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I9"/>
       <c r="J9"/>
       <c r="K9"/>
       <c r="L9" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M9"/>
       <c r="N9"/>
       <c r="O9" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="P9"/>
       <c r="Q9"/>
@@ -942,16 +971,16 @@
       <c r="S9"/>
       <c r="T9"/>
     </row>
-    <row r="10" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
       <c r="F10" s="13"/>
       <c r="G10" s="13"/>
-      <c r="H10" s="20" t="s">
-        <v>20</v>
+      <c r="H10" s="18" t="s">
+        <v>19</v>
       </c>
       <c r="I10"/>
       <c r="J10"/>
@@ -966,101 +995,101 @@
       <c r="S10"/>
       <c r="T10"/>
     </row>
-    <row r="11" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="17"/>
+    <row r="11" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="15"/>
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
       <c r="H11" s="14"/>
     </row>
-    <row r="12" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="17"/>
+    <row r="12" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="15"/>
       <c r="F12" s="13"/>
       <c r="G12" s="13"/>
       <c r="H12" s="14"/>
     </row>
-    <row r="13" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="17"/>
+    <row r="13" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="15"/>
       <c r="F13" s="13"/>
       <c r="G13" s="13"/>
       <c r="H13" s="14"/>
     </row>
-    <row r="14" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="17"/>
+    <row r="14" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="15"/>
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
       <c r="H14" s="7"/>
     </row>
-    <row r="15" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="17"/>
+    <row r="15" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="15"/>
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
       <c r="H15" s="7"/>
     </row>
-    <row r="16" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="17"/>
+    <row r="16" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="15"/>
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
       <c r="H16" s="7"/>
     </row>
-    <row r="17" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="17"/>
+    <row r="17" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="15"/>
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>
       <c r="H17" s="7"/>
     </row>
-    <row r="18" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="17"/>
+    <row r="18" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="15"/>
       <c r="F18" s="7"/>
       <c r="G18" s="7"/>
       <c r="H18" s="7"/>
     </row>
-    <row r="19" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="17"/>
+    <row r="19" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="15"/>
       <c r="F19" s="7"/>
       <c r="G19" s="7"/>
       <c r="H19" s="7"/>
     </row>
-    <row r="20" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="17"/>
+    <row r="20" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="15"/>
       <c r="F20" s="7"/>
       <c r="G20" s="7"/>
       <c r="H20" s="7"/>
     </row>
-    <row r="21" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="17"/>
-      <c r="C21" s="17"/>
+    <row r="21" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="15"/>
+      <c r="C21" s="15"/>
       <c r="F21" s="7"/>
       <c r="G21" s="7"/>
       <c r="H21" s="7"/>
     </row>
-    <row r="22" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="17"/>
-      <c r="C22" s="17"/>
+    <row r="22" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="15"/>
+      <c r="C22" s="15"/>
       <c r="F22" s="7"/>
       <c r="G22" s="7"/>
       <c r="H22" s="7"/>
     </row>
-    <row r="23" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="17"/>
+    <row r="23" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="15"/>
       <c r="F23" s="7"/>
       <c r="G23" s="7"/>
       <c r="H23" s="7"/>
     </row>
-    <row r="24" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="17"/>
+    <row r="24" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="15"/>
       <c r="F24" s="7"/>
       <c r="G24" s="7"/>
       <c r="H24" s="7"/>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A25" s="17"/>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A25" s="15"/>
       <c r="B25" s="6"/>
-      <c r="C25" s="17"/>
+      <c r="C25" s="15"/>
       <c r="D25" s="6"/>
       <c r="E25" s="6"/>
       <c r="F25" s="6"/>
       <c r="G25" s="6"/>
-      <c r="H25" s="18"/>
+      <c r="H25" s="16"/>
       <c r="I25" s="6"/>
       <c r="J25" s="6"/>
       <c r="K25" s="6"/>
@@ -1074,15 +1103,15 @@
       <c r="S25" s="6"/>
       <c r="T25" s="6"/>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A26" s="17"/>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A26" s="15"/>
       <c r="B26" s="6"/>
-      <c r="C26" s="17"/>
+      <c r="C26" s="15"/>
       <c r="D26" s="6"/>
       <c r="E26" s="6"/>
       <c r="F26" s="6"/>
       <c r="G26" s="6"/>
-      <c r="H26" s="18"/>
+      <c r="H26" s="16"/>
       <c r="I26" s="6"/>
       <c r="J26" s="6"/>
       <c r="K26" s="6"/>
@@ -1097,18 +1126,23 @@
       <c r="T26" s="6"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C21:C24 A21:A24 C4:D8 C9:C13 A4:A13">
-    <cfRule type="cellIs" dxfId="14" priority="3" operator="equal">
+  <conditionalFormatting sqref="C21:C24 A21:A24 C4:D5 C9:C13 A4:A5 A7:A13 C7:D8">
+    <cfRule type="cellIs" dxfId="19" priority="4" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A26">
-    <cfRule type="cellIs" dxfId="13" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="2" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A25">
-    <cfRule type="cellIs" dxfId="12" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="3" operator="equal">
+      <formula>"class"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C6:D6 A6">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1125,23 +1159,24 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H2" sqref="H2"/>
+      <selection activeCell="K22" sqref="K22"/>
+      <selection pane="topRight" activeCell="K22" sqref="K22"/>
+      <selection pane="bottomLeft" activeCell="K22" sqref="K22"/>
+      <selection pane="bottomRight" activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" style="19" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" style="17" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
     <col min="6" max="8" width="10" customWidth="1"/>
-    <col min="9" max="15" width="6.6640625" customWidth="1"/>
+    <col min="9" max="15" width="6.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
@@ -1161,7 +1196,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -1170,8 +1205,8 @@
       <c r="E2" s="7"/>
       <c r="F2" s="7"/>
       <c r="G2" s="7"/>
-      <c r="H2" s="21" t="s">
-        <v>28</v>
+      <c r="H2" s="19" t="s">
+        <v>27</v>
       </c>
       <c r="I2"/>
       <c r="J2"/>
@@ -1192,7 +1227,7 @@
       <c r="Z2"/>
       <c r="AA2"/>
     </row>
-    <row r="3" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
@@ -1201,7 +1236,7 @@
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
       <c r="H3" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I3"/>
       <c r="J3"/>
@@ -1222,7 +1257,7 @@
       <c r="Z3"/>
       <c r="AA3"/>
     </row>
-    <row r="4" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>7</v>
       </c>
@@ -1253,15 +1288,15 @@
       <c r="Z4"/>
       <c r="AA4"/>
     </row>
-    <row r="5" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
       <c r="G5" s="13"/>
-      <c r="H5" s="20" t="s">
-        <v>25</v>
+      <c r="H5" s="18" t="s">
+        <v>24</v>
       </c>
       <c r="J5"/>
       <c r="K5"/>
@@ -1282,49 +1317,37 @@
       <c r="Z5"/>
       <c r="AA5"/>
     </row>
-    <row r="6" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
-      <c r="F6" s="15">
-        <v>10</v>
-      </c>
-      <c r="G6" s="16">
-        <v>1</v>
-      </c>
-      <c r="H6" s="16">
-        <v>2</v>
-      </c>
-      <c r="J6"/>
-      <c r="K6"/>
-      <c r="L6"/>
-      <c r="M6"/>
-      <c r="N6"/>
-      <c r="O6"/>
-      <c r="P6"/>
-      <c r="Q6"/>
-      <c r="R6"/>
-      <c r="S6"/>
-      <c r="T6"/>
-      <c r="U6"/>
-      <c r="V6"/>
-      <c r="W6"/>
-      <c r="X6"/>
-      <c r="Y6"/>
-      <c r="Z6"/>
-      <c r="AA6"/>
-    </row>
-    <row r="7" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" s="20">
+        <v>0</v>
+      </c>
+      <c r="G6" s="21">
+        <v>0</v>
+      </c>
+      <c r="H6" s="21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
       <c r="G7" s="13"/>
-      <c r="H7" s="20" t="s">
-        <v>13</v>
+      <c r="H7" s="18" t="s">
+        <v>12</v>
       </c>
       <c r="J7"/>
       <c r="K7"/>
@@ -1345,15 +1368,15 @@
       <c r="Z7"/>
       <c r="AA7"/>
     </row>
-    <row r="8" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
       <c r="G8" s="13"/>
-      <c r="H8" s="20" t="s">
-        <v>15</v>
+      <c r="H8" s="18" t="s">
+        <v>14</v>
       </c>
       <c r="J8"/>
       <c r="K8"/>
@@ -1374,27 +1397,27 @@
       <c r="Z8"/>
       <c r="AA8"/>
     </row>
-    <row r="9" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
       <c r="F9" s="13"/>
       <c r="G9" s="13"/>
       <c r="H9" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I9"/>
       <c r="J9"/>
       <c r="K9"/>
       <c r="L9" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M9"/>
       <c r="N9"/>
       <c r="O9" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="P9"/>
       <c r="Q9"/>
@@ -1402,16 +1425,16 @@
       <c r="S9"/>
       <c r="T9"/>
     </row>
-    <row r="10" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
       <c r="F10" s="13"/>
       <c r="G10" s="13"/>
-      <c r="H10" s="20" t="s">
-        <v>20</v>
+      <c r="H10" s="18" t="s">
+        <v>19</v>
       </c>
       <c r="I10"/>
       <c r="J10"/>
@@ -1426,101 +1449,101 @@
       <c r="S10"/>
       <c r="T10"/>
     </row>
-    <row r="11" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="17"/>
+    <row r="11" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="15"/>
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
       <c r="H11" s="14"/>
     </row>
-    <row r="12" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="17"/>
+    <row r="12" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="15"/>
       <c r="F12" s="13"/>
       <c r="G12" s="13"/>
       <c r="H12" s="14"/>
     </row>
-    <row r="13" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="17"/>
+    <row r="13" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="15"/>
       <c r="F13" s="13"/>
       <c r="G13" s="13"/>
       <c r="H13" s="14"/>
     </row>
-    <row r="14" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="17"/>
+    <row r="14" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="15"/>
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
       <c r="H14" s="7"/>
     </row>
-    <row r="15" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="17"/>
+    <row r="15" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="15"/>
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
       <c r="H15" s="7"/>
     </row>
-    <row r="16" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="17"/>
+    <row r="16" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="15"/>
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
       <c r="H16" s="7"/>
     </row>
-    <row r="17" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="17"/>
+    <row r="17" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="15"/>
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>
       <c r="H17" s="7"/>
     </row>
-    <row r="18" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="17"/>
+    <row r="18" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="15"/>
       <c r="F18" s="7"/>
       <c r="G18" s="7"/>
       <c r="H18" s="7"/>
     </row>
-    <row r="19" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="17"/>
+    <row r="19" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="15"/>
       <c r="F19" s="7"/>
       <c r="G19" s="7"/>
       <c r="H19" s="7"/>
     </row>
-    <row r="20" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="17"/>
+    <row r="20" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="15"/>
       <c r="F20" s="7"/>
       <c r="G20" s="7"/>
       <c r="H20" s="7"/>
     </row>
-    <row r="21" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="17"/>
-      <c r="C21" s="17"/>
+    <row r="21" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="15"/>
+      <c r="C21" s="15"/>
       <c r="F21" s="7"/>
       <c r="G21" s="7"/>
       <c r="H21" s="7"/>
     </row>
-    <row r="22" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="17"/>
-      <c r="C22" s="17"/>
+    <row r="22" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="15"/>
+      <c r="C22" s="15"/>
       <c r="F22" s="7"/>
       <c r="G22" s="7"/>
       <c r="H22" s="7"/>
     </row>
-    <row r="23" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="17"/>
+    <row r="23" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="15"/>
       <c r="F23" s="7"/>
       <c r="G23" s="7"/>
       <c r="H23" s="7"/>
     </row>
-    <row r="24" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="17"/>
+    <row r="24" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="15"/>
       <c r="F24" s="7"/>
       <c r="G24" s="7"/>
       <c r="H24" s="7"/>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A25" s="17"/>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A25" s="15"/>
       <c r="B25" s="6"/>
-      <c r="C25" s="17"/>
+      <c r="C25" s="15"/>
       <c r="D25" s="6"/>
       <c r="E25" s="6"/>
       <c r="F25" s="6"/>
       <c r="G25" s="6"/>
-      <c r="H25" s="18"/>
+      <c r="H25" s="16"/>
       <c r="I25" s="6"/>
       <c r="J25" s="6"/>
       <c r="K25" s="6"/>
@@ -1534,15 +1557,15 @@
       <c r="S25" s="6"/>
       <c r="T25" s="6"/>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A26" s="17"/>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A26" s="15"/>
       <c r="B26" s="6"/>
-      <c r="C26" s="17"/>
+      <c r="C26" s="15"/>
       <c r="D26" s="6"/>
       <c r="E26" s="6"/>
       <c r="F26" s="6"/>
       <c r="G26" s="6"/>
-      <c r="H26" s="18"/>
+      <c r="H26" s="16"/>
       <c r="I26" s="6"/>
       <c r="J26" s="6"/>
       <c r="K26" s="6"/>
@@ -1557,18 +1580,23 @@
       <c r="T26" s="6"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C21:C24 A21:A24 C4:D8 C9:C13 A4:A13">
-    <cfRule type="cellIs" dxfId="11" priority="3" operator="equal">
+  <conditionalFormatting sqref="C21:C24 A21:A24 C4:D5 C9:C13 A4:A5 A7:A13 C7:D8">
+    <cfRule type="cellIs" dxfId="16" priority="4" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A26">
-    <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="2" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A25">
-    <cfRule type="cellIs" dxfId="9" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="3" operator="equal">
+      <formula>"class"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C6:D6 A6">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1585,23 +1613,24 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H2" sqref="H2"/>
+      <selection activeCell="K22" sqref="K22"/>
+      <selection pane="topRight" activeCell="K22" sqref="K22"/>
+      <selection pane="bottomLeft" activeCell="K22" sqref="K22"/>
+      <selection pane="bottomRight" activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" style="19" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" style="17" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
     <col min="6" max="8" width="10" customWidth="1"/>
-    <col min="9" max="15" width="6.6640625" customWidth="1"/>
+    <col min="9" max="15" width="6.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
@@ -1621,7 +1650,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -1630,8 +1659,8 @@
       <c r="E2" s="7"/>
       <c r="F2" s="7"/>
       <c r="G2" s="7"/>
-      <c r="H2" s="21" t="s">
-        <v>28</v>
+      <c r="H2" s="19" t="s">
+        <v>27</v>
       </c>
       <c r="I2"/>
       <c r="J2"/>
@@ -1652,7 +1681,7 @@
       <c r="Z2"/>
       <c r="AA2"/>
     </row>
-    <row r="3" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
@@ -1661,7 +1690,7 @@
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
       <c r="H3" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I3"/>
       <c r="J3"/>
@@ -1682,7 +1711,7 @@
       <c r="Z3"/>
       <c r="AA3"/>
     </row>
-    <row r="4" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>7</v>
       </c>
@@ -1713,15 +1742,15 @@
       <c r="Z4"/>
       <c r="AA4"/>
     </row>
-    <row r="5" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
       <c r="G5" s="13"/>
-      <c r="H5" s="20" t="s">
-        <v>23</v>
+      <c r="H5" s="18" t="s">
+        <v>22</v>
       </c>
       <c r="J5"/>
       <c r="K5"/>
@@ -1742,49 +1771,37 @@
       <c r="Z5"/>
       <c r="AA5"/>
     </row>
-    <row r="6" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
-      <c r="F6" s="15">
-        <v>10</v>
-      </c>
-      <c r="G6" s="16">
-        <v>1</v>
-      </c>
-      <c r="H6" s="16">
-        <v>2</v>
-      </c>
-      <c r="J6"/>
-      <c r="K6"/>
-      <c r="L6"/>
-      <c r="M6"/>
-      <c r="N6"/>
-      <c r="O6"/>
-      <c r="P6"/>
-      <c r="Q6"/>
-      <c r="R6"/>
-      <c r="S6"/>
-      <c r="T6"/>
-      <c r="U6"/>
-      <c r="V6"/>
-      <c r="W6"/>
-      <c r="X6"/>
-      <c r="Y6"/>
-      <c r="Z6"/>
-      <c r="AA6"/>
-    </row>
-    <row r="7" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" s="20">
+        <v>0</v>
+      </c>
+      <c r="G6" s="21">
+        <v>0</v>
+      </c>
+      <c r="H6" s="21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
       <c r="G7" s="13"/>
-      <c r="H7" s="20" t="s">
-        <v>13</v>
+      <c r="H7" s="18" t="s">
+        <v>12</v>
       </c>
       <c r="J7"/>
       <c r="K7"/>
@@ -1805,15 +1822,15 @@
       <c r="Z7"/>
       <c r="AA7"/>
     </row>
-    <row r="8" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
       <c r="G8" s="13"/>
-      <c r="H8" s="20" t="s">
-        <v>15</v>
+      <c r="H8" s="18" t="s">
+        <v>14</v>
       </c>
       <c r="J8"/>
       <c r="K8"/>
@@ -1834,27 +1851,27 @@
       <c r="Z8"/>
       <c r="AA8"/>
     </row>
-    <row r="9" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
       <c r="F9" s="13"/>
       <c r="G9" s="13"/>
       <c r="H9" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I9"/>
       <c r="J9"/>
       <c r="K9"/>
       <c r="L9" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M9"/>
       <c r="N9"/>
       <c r="O9" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="P9"/>
       <c r="Q9"/>
@@ -1862,16 +1879,16 @@
       <c r="S9"/>
       <c r="T9"/>
     </row>
-    <row r="10" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
       <c r="F10" s="13"/>
       <c r="G10" s="13"/>
-      <c r="H10" s="20" t="s">
-        <v>20</v>
+      <c r="H10" s="18" t="s">
+        <v>19</v>
       </c>
       <c r="I10"/>
       <c r="J10"/>
@@ -1886,101 +1903,101 @@
       <c r="S10"/>
       <c r="T10"/>
     </row>
-    <row r="11" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="17"/>
+    <row r="11" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="15"/>
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
       <c r="H11" s="14"/>
     </row>
-    <row r="12" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="17"/>
+    <row r="12" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="15"/>
       <c r="F12" s="13"/>
       <c r="G12" s="13"/>
       <c r="H12" s="14"/>
     </row>
-    <row r="13" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="17"/>
+    <row r="13" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="15"/>
       <c r="F13" s="13"/>
       <c r="G13" s="13"/>
       <c r="H13" s="14"/>
     </row>
-    <row r="14" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="17"/>
+    <row r="14" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="15"/>
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
       <c r="H14" s="7"/>
     </row>
-    <row r="15" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="17"/>
+    <row r="15" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="15"/>
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
       <c r="H15" s="7"/>
     </row>
-    <row r="16" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="17"/>
+    <row r="16" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="15"/>
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
       <c r="H16" s="7"/>
     </row>
-    <row r="17" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="17"/>
+    <row r="17" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="15"/>
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>
       <c r="H17" s="7"/>
     </row>
-    <row r="18" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="17"/>
+    <row r="18" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="15"/>
       <c r="F18" s="7"/>
       <c r="G18" s="7"/>
       <c r="H18" s="7"/>
     </row>
-    <row r="19" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="17"/>
+    <row r="19" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="15"/>
       <c r="F19" s="7"/>
       <c r="G19" s="7"/>
       <c r="H19" s="7"/>
     </row>
-    <row r="20" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="17"/>
+    <row r="20" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="15"/>
       <c r="F20" s="7"/>
       <c r="G20" s="7"/>
       <c r="H20" s="7"/>
     </row>
-    <row r="21" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="17"/>
-      <c r="C21" s="17"/>
+    <row r="21" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="15"/>
+      <c r="C21" s="15"/>
       <c r="F21" s="7"/>
       <c r="G21" s="7"/>
       <c r="H21" s="7"/>
     </row>
-    <row r="22" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="17"/>
-      <c r="C22" s="17"/>
+    <row r="22" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="15"/>
+      <c r="C22" s="15"/>
       <c r="F22" s="7"/>
       <c r="G22" s="7"/>
       <c r="H22" s="7"/>
     </row>
-    <row r="23" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="17"/>
+    <row r="23" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="15"/>
       <c r="F23" s="7"/>
       <c r="G23" s="7"/>
       <c r="H23" s="7"/>
     </row>
-    <row r="24" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="17"/>
+    <row r="24" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="15"/>
       <c r="F24" s="7"/>
       <c r="G24" s="7"/>
       <c r="H24" s="7"/>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A25" s="17"/>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A25" s="15"/>
       <c r="B25" s="6"/>
-      <c r="C25" s="17"/>
+      <c r="C25" s="15"/>
       <c r="D25" s="6"/>
       <c r="E25" s="6"/>
       <c r="F25" s="6"/>
       <c r="G25" s="6"/>
-      <c r="H25" s="18"/>
+      <c r="H25" s="16"/>
       <c r="I25" s="6"/>
       <c r="J25" s="6"/>
       <c r="K25" s="6"/>
@@ -1994,15 +2011,15 @@
       <c r="S25" s="6"/>
       <c r="T25" s="6"/>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A26" s="17"/>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A26" s="15"/>
       <c r="B26" s="6"/>
-      <c r="C26" s="17"/>
+      <c r="C26" s="15"/>
       <c r="D26" s="6"/>
       <c r="E26" s="6"/>
       <c r="F26" s="6"/>
       <c r="G26" s="6"/>
-      <c r="H26" s="18"/>
+      <c r="H26" s="16"/>
       <c r="I26" s="6"/>
       <c r="J26" s="6"/>
       <c r="K26" s="6"/>
@@ -2017,18 +2034,23 @@
       <c r="T26" s="6"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C21:C24 A21:A24 C4:D8 C9:C13 A4:A13">
-    <cfRule type="cellIs" dxfId="8" priority="3" operator="equal">
+  <conditionalFormatting sqref="C21:C24 A21:A24 C4:D5 C9:C13 A4:A5 A7:A13 C7:D8">
+    <cfRule type="cellIs" dxfId="13" priority="4" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A26">
-    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="2" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A25">
-    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="3" operator="equal">
+      <formula>"class"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C6:D6 A6">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2045,23 +2067,24 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H2" sqref="H2"/>
+      <selection activeCell="K22" sqref="K22"/>
+      <selection pane="topRight" activeCell="K22" sqref="K22"/>
+      <selection pane="bottomLeft" activeCell="K22" sqref="K22"/>
+      <selection pane="bottomRight" activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" style="19" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" style="17" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
     <col min="6" max="8" width="10" customWidth="1"/>
-    <col min="9" max="15" width="6.6640625" customWidth="1"/>
+    <col min="9" max="15" width="6.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
@@ -2081,7 +2104,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -2090,8 +2113,8 @@
       <c r="E2" s="7"/>
       <c r="F2" s="7"/>
       <c r="G2" s="7"/>
-      <c r="H2" s="21" t="s">
-        <v>28</v>
+      <c r="H2" s="19" t="s">
+        <v>27</v>
       </c>
       <c r="I2"/>
       <c r="J2"/>
@@ -2112,7 +2135,7 @@
       <c r="Z2"/>
       <c r="AA2"/>
     </row>
-    <row r="3" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
@@ -2121,7 +2144,7 @@
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
       <c r="H3" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I3"/>
       <c r="J3"/>
@@ -2142,7 +2165,7 @@
       <c r="Z3"/>
       <c r="AA3"/>
     </row>
-    <row r="4" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>7</v>
       </c>
@@ -2173,15 +2196,15 @@
       <c r="Z4"/>
       <c r="AA4"/>
     </row>
-    <row r="5" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
       <c r="G5" s="13"/>
-      <c r="H5" s="20" t="s">
-        <v>27</v>
+      <c r="H5" s="18" t="s">
+        <v>26</v>
       </c>
       <c r="J5"/>
       <c r="K5"/>
@@ -2202,49 +2225,37 @@
       <c r="Z5"/>
       <c r="AA5"/>
     </row>
-    <row r="6" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
-      <c r="F6" s="15">
-        <v>10</v>
-      </c>
-      <c r="G6" s="16">
-        <v>1</v>
-      </c>
-      <c r="H6" s="16">
-        <v>2</v>
-      </c>
-      <c r="J6"/>
-      <c r="K6"/>
-      <c r="L6"/>
-      <c r="M6"/>
-      <c r="N6"/>
-      <c r="O6"/>
-      <c r="P6"/>
-      <c r="Q6"/>
-      <c r="R6"/>
-      <c r="S6"/>
-      <c r="T6"/>
-      <c r="U6"/>
-      <c r="V6"/>
-      <c r="W6"/>
-      <c r="X6"/>
-      <c r="Y6"/>
-      <c r="Z6"/>
-      <c r="AA6"/>
-    </row>
-    <row r="7" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" s="20">
+        <v>0</v>
+      </c>
+      <c r="G6" s="21">
+        <v>0</v>
+      </c>
+      <c r="H6" s="21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
       <c r="G7" s="13"/>
-      <c r="H7" s="20" t="s">
-        <v>13</v>
+      <c r="H7" s="18" t="s">
+        <v>12</v>
       </c>
       <c r="J7"/>
       <c r="K7"/>
@@ -2265,15 +2276,15 @@
       <c r="Z7"/>
       <c r="AA7"/>
     </row>
-    <row r="8" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
       <c r="G8" s="13"/>
-      <c r="H8" s="20" t="s">
-        <v>15</v>
+      <c r="H8" s="18" t="s">
+        <v>14</v>
       </c>
       <c r="J8"/>
       <c r="K8"/>
@@ -2294,27 +2305,27 @@
       <c r="Z8"/>
       <c r="AA8"/>
     </row>
-    <row r="9" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
       <c r="F9" s="13"/>
       <c r="G9" s="13"/>
       <c r="H9" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I9"/>
       <c r="J9"/>
       <c r="K9"/>
       <c r="L9" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M9"/>
       <c r="N9"/>
       <c r="O9" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="P9"/>
       <c r="Q9"/>
@@ -2322,16 +2333,16 @@
       <c r="S9"/>
       <c r="T9"/>
     </row>
-    <row r="10" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
       <c r="F10" s="13"/>
       <c r="G10" s="13"/>
-      <c r="H10" s="20" t="s">
-        <v>20</v>
+      <c r="H10" s="18" t="s">
+        <v>19</v>
       </c>
       <c r="I10"/>
       <c r="J10"/>
@@ -2346,101 +2357,101 @@
       <c r="S10"/>
       <c r="T10"/>
     </row>
-    <row r="11" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="17"/>
+    <row r="11" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="15"/>
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
       <c r="H11" s="14"/>
     </row>
-    <row r="12" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="17"/>
+    <row r="12" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="15"/>
       <c r="F12" s="13"/>
       <c r="G12" s="13"/>
       <c r="H12" s="14"/>
     </row>
-    <row r="13" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="17"/>
+    <row r="13" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="15"/>
       <c r="F13" s="13"/>
       <c r="G13" s="13"/>
       <c r="H13" s="14"/>
     </row>
-    <row r="14" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="17"/>
+    <row r="14" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="15"/>
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
       <c r="H14" s="7"/>
     </row>
-    <row r="15" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="17"/>
+    <row r="15" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="15"/>
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
       <c r="H15" s="7"/>
     </row>
-    <row r="16" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="17"/>
+    <row r="16" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="15"/>
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
       <c r="H16" s="7"/>
     </row>
-    <row r="17" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="17"/>
+    <row r="17" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="15"/>
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>
       <c r="H17" s="7"/>
     </row>
-    <row r="18" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="17"/>
+    <row r="18" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="15"/>
       <c r="F18" s="7"/>
       <c r="G18" s="7"/>
       <c r="H18" s="7"/>
     </row>
-    <row r="19" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="17"/>
+    <row r="19" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="15"/>
       <c r="F19" s="7"/>
       <c r="G19" s="7"/>
       <c r="H19" s="7"/>
     </row>
-    <row r="20" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="17"/>
+    <row r="20" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="15"/>
       <c r="F20" s="7"/>
       <c r="G20" s="7"/>
       <c r="H20" s="7"/>
     </row>
-    <row r="21" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="17"/>
-      <c r="C21" s="17"/>
+    <row r="21" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="15"/>
+      <c r="C21" s="15"/>
       <c r="F21" s="7"/>
       <c r="G21" s="7"/>
       <c r="H21" s="7"/>
     </row>
-    <row r="22" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="17"/>
-      <c r="C22" s="17"/>
+    <row r="22" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="15"/>
+      <c r="C22" s="15"/>
       <c r="F22" s="7"/>
       <c r="G22" s="7"/>
       <c r="H22" s="7"/>
     </row>
-    <row r="23" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="17"/>
+    <row r="23" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="15"/>
       <c r="F23" s="7"/>
       <c r="G23" s="7"/>
       <c r="H23" s="7"/>
     </row>
-    <row r="24" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="17"/>
+    <row r="24" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="15"/>
       <c r="F24" s="7"/>
       <c r="G24" s="7"/>
       <c r="H24" s="7"/>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A25" s="17"/>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A25" s="15"/>
       <c r="B25" s="6"/>
-      <c r="C25" s="17"/>
+      <c r="C25" s="15"/>
       <c r="D25" s="6"/>
       <c r="E25" s="6"/>
       <c r="F25" s="6"/>
       <c r="G25" s="6"/>
-      <c r="H25" s="18"/>
+      <c r="H25" s="16"/>
       <c r="I25" s="6"/>
       <c r="J25" s="6"/>
       <c r="K25" s="6"/>
@@ -2454,15 +2465,15 @@
       <c r="S25" s="6"/>
       <c r="T25" s="6"/>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A26" s="17"/>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A26" s="15"/>
       <c r="B26" s="6"/>
-      <c r="C26" s="17"/>
+      <c r="C26" s="15"/>
       <c r="D26" s="6"/>
       <c r="E26" s="6"/>
       <c r="F26" s="6"/>
       <c r="G26" s="6"/>
-      <c r="H26" s="18"/>
+      <c r="H26" s="16"/>
       <c r="I26" s="6"/>
       <c r="J26" s="6"/>
       <c r="K26" s="6"/>
@@ -2477,18 +2488,23 @@
       <c r="T26" s="6"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C21:C24 A21:A24 C4:D8 C9:C13 A4:A13">
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+  <conditionalFormatting sqref="C21:C24 A21:A24 C4:D5 C9:C13 A4:A5 A7:A13 C7:D8">
+    <cfRule type="cellIs" dxfId="10" priority="4" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A26">
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="2" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A25">
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="3" operator="equal">
+      <formula>"class"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C6:D6 A6">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2503,25 +2519,25 @@
   </sheetPr>
   <dimension ref="A1:AA26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H6" sqref="H6"/>
+      <selection pane="bottomRight" activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" style="19" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" style="17" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
     <col min="6" max="8" width="10" customWidth="1"/>
-    <col min="9" max="15" width="6.6640625" customWidth="1"/>
+    <col min="9" max="15" width="6.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
@@ -2541,7 +2557,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -2550,8 +2566,8 @@
       <c r="E2" s="7"/>
       <c r="F2" s="7"/>
       <c r="G2" s="7"/>
-      <c r="H2" s="21" t="s">
-        <v>28</v>
+      <c r="H2" s="19" t="s">
+        <v>27</v>
       </c>
       <c r="I2"/>
       <c r="J2"/>
@@ -2572,7 +2588,7 @@
       <c r="Z2"/>
       <c r="AA2"/>
     </row>
-    <row r="3" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
@@ -2581,7 +2597,7 @@
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
       <c r="H3" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I3"/>
       <c r="J3"/>
@@ -2602,7 +2618,7 @@
       <c r="Z3"/>
       <c r="AA3"/>
     </row>
-    <row r="4" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>7</v>
       </c>
@@ -2633,15 +2649,15 @@
       <c r="Z4"/>
       <c r="AA4"/>
     </row>
-    <row r="5" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
       <c r="G5" s="13"/>
-      <c r="H5" s="20" t="s">
-        <v>31</v>
+      <c r="H5" s="18" t="s">
+        <v>30</v>
       </c>
       <c r="J5"/>
       <c r="K5"/>
@@ -2662,49 +2678,37 @@
       <c r="Z5"/>
       <c r="AA5"/>
     </row>
-    <row r="6" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
-      <c r="F6" s="15">
-        <v>10</v>
-      </c>
-      <c r="G6" s="16">
-        <v>1</v>
-      </c>
-      <c r="H6" s="16">
-        <v>2</v>
-      </c>
-      <c r="J6"/>
-      <c r="K6"/>
-      <c r="L6"/>
-      <c r="M6"/>
-      <c r="N6"/>
-      <c r="O6"/>
-      <c r="P6"/>
-      <c r="Q6"/>
-      <c r="R6"/>
-      <c r="S6"/>
-      <c r="T6"/>
-      <c r="U6"/>
-      <c r="V6"/>
-      <c r="W6"/>
-      <c r="X6"/>
-      <c r="Y6"/>
-      <c r="Z6"/>
-      <c r="AA6"/>
-    </row>
-    <row r="7" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" s="20">
+        <v>0</v>
+      </c>
+      <c r="G6" s="21">
+        <v>0</v>
+      </c>
+      <c r="H6" s="21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
       <c r="G7" s="13"/>
-      <c r="H7" s="20" t="s">
-        <v>13</v>
+      <c r="H7" s="18" t="s">
+        <v>12</v>
       </c>
       <c r="J7"/>
       <c r="K7"/>
@@ -2725,15 +2729,15 @@
       <c r="Z7"/>
       <c r="AA7"/>
     </row>
-    <row r="8" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
       <c r="G8" s="13"/>
-      <c r="H8" s="20" t="s">
-        <v>15</v>
+      <c r="H8" s="18" t="s">
+        <v>14</v>
       </c>
       <c r="J8"/>
       <c r="K8"/>
@@ -2754,27 +2758,27 @@
       <c r="Z8"/>
       <c r="AA8"/>
     </row>
-    <row r="9" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
       <c r="F9" s="13"/>
       <c r="G9" s="13"/>
       <c r="H9" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I9"/>
       <c r="J9"/>
       <c r="K9"/>
       <c r="L9" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M9"/>
       <c r="N9"/>
       <c r="O9" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="P9"/>
       <c r="Q9"/>
@@ -2782,16 +2786,16 @@
       <c r="S9"/>
       <c r="T9"/>
     </row>
-    <row r="10" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
       <c r="F10" s="13"/>
       <c r="G10" s="13"/>
-      <c r="H10" s="20" t="s">
-        <v>20</v>
+      <c r="H10" s="18" t="s">
+        <v>19</v>
       </c>
       <c r="I10"/>
       <c r="J10"/>
@@ -2806,101 +2810,101 @@
       <c r="S10"/>
       <c r="T10"/>
     </row>
-    <row r="11" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="17"/>
+    <row r="11" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="15"/>
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
       <c r="H11" s="14"/>
     </row>
-    <row r="12" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="17"/>
+    <row r="12" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="15"/>
       <c r="F12" s="13"/>
       <c r="G12" s="13"/>
       <c r="H12" s="14"/>
     </row>
-    <row r="13" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="17"/>
+    <row r="13" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="15"/>
       <c r="F13" s="13"/>
       <c r="G13" s="13"/>
       <c r="H13" s="14"/>
     </row>
-    <row r="14" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="17"/>
+    <row r="14" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="15"/>
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
       <c r="H14" s="7"/>
     </row>
-    <row r="15" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="17"/>
+    <row r="15" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="15"/>
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
       <c r="H15" s="7"/>
     </row>
-    <row r="16" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="17"/>
+    <row r="16" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="15"/>
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
       <c r="H16" s="7"/>
     </row>
-    <row r="17" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="17"/>
+    <row r="17" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="15"/>
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>
       <c r="H17" s="7"/>
     </row>
-    <row r="18" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="17"/>
+    <row r="18" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="15"/>
       <c r="F18" s="7"/>
       <c r="G18" s="7"/>
       <c r="H18" s="7"/>
     </row>
-    <row r="19" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="17"/>
+    <row r="19" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="15"/>
       <c r="F19" s="7"/>
       <c r="G19" s="7"/>
       <c r="H19" s="7"/>
     </row>
-    <row r="20" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="17"/>
+    <row r="20" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="15"/>
       <c r="F20" s="7"/>
       <c r="G20" s="7"/>
       <c r="H20" s="7"/>
     </row>
-    <row r="21" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="17"/>
-      <c r="C21" s="17"/>
+    <row r="21" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="15"/>
+      <c r="C21" s="15"/>
       <c r="F21" s="7"/>
       <c r="G21" s="7"/>
       <c r="H21" s="7"/>
     </row>
-    <row r="22" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="17"/>
-      <c r="C22" s="17"/>
+    <row r="22" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="15"/>
+      <c r="C22" s="15"/>
       <c r="F22" s="7"/>
       <c r="G22" s="7"/>
       <c r="H22" s="7"/>
     </row>
-    <row r="23" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="17"/>
+    <row r="23" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="15"/>
       <c r="F23" s="7"/>
       <c r="G23" s="7"/>
       <c r="H23" s="7"/>
     </row>
-    <row r="24" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="17"/>
+    <row r="24" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="15"/>
       <c r="F24" s="7"/>
       <c r="G24" s="7"/>
       <c r="H24" s="7"/>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A25" s="17"/>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A25" s="15"/>
       <c r="B25" s="6"/>
-      <c r="C25" s="17"/>
+      <c r="C25" s="15"/>
       <c r="D25" s="6"/>
       <c r="E25" s="6"/>
       <c r="F25" s="6"/>
       <c r="G25" s="6"/>
-      <c r="H25" s="18"/>
+      <c r="H25" s="16"/>
       <c r="I25" s="6"/>
       <c r="J25" s="6"/>
       <c r="K25" s="6"/>
@@ -2914,15 +2918,15 @@
       <c r="S25" s="6"/>
       <c r="T25" s="6"/>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A26" s="17"/>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A26" s="15"/>
       <c r="B26" s="6"/>
-      <c r="C26" s="17"/>
+      <c r="C26" s="15"/>
       <c r="D26" s="6"/>
       <c r="E26" s="6"/>
       <c r="F26" s="6"/>
       <c r="G26" s="6"/>
-      <c r="H26" s="18"/>
+      <c r="H26" s="16"/>
       <c r="I26" s="6"/>
       <c r="J26" s="6"/>
       <c r="K26" s="6"/>
@@ -2937,18 +2941,23 @@
       <c r="T26" s="6"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C21:C24 A21:A24 C4:D8 C9:C13 A4:A13">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+  <conditionalFormatting sqref="C21:C24 A21:A24 C4:D5 C9:C13 A4:A5 A7:A13 C7:D8">
+    <cfRule type="cellIs" dxfId="7" priority="4" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A26">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A25">
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+      <formula>"class"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C6:D6 A6">
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>